<commit_message>
reset password page done
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="111">
   <si>
     <t>user id</t>
   </si>
@@ -344,25 +344,28 @@
     <t>ori</t>
   </si>
   <si>
-    <t>e923f97cfc6829bdf5bde80f6662b765e14c3e5fc7520433a869d6eb652750c6</t>
-  </si>
-  <si>
-    <t>fce44a7d7b602fbcf9c9fd96734ee6a2f86acfd8d405dd146b52049f093e10ff</t>
-  </si>
-  <si>
-    <t>a7a723a7902c677aab6417925b80a5c3b9ea9934394f755b1afb9debd9c0c021</t>
-  </si>
-  <si>
-    <t>1d83ec315945d0b8bea3b21e3df2d1d3d137794ec779b4bce948eba820b34c41</t>
-  </si>
-  <si>
-    <t>d45b338dfdfa2eccd465836cd68cf5d9cdee5d55eb7eb45558a95bc2c0cb1e69</t>
-  </si>
-  <si>
     <t>file</t>
   </si>
   <si>
     <t>command</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>5cdaa7c6ef937092cf5c07b3ff99eb6990a706ba5f1ae4cf7b1129438f63283b</t>
+  </si>
+  <si>
+    <t>37fda81a029841c400e28e6a226bb42c274dcf95f11e23a3b71f98c3ed21f6fa</t>
+  </si>
+  <si>
+    <t>397058f7e63d4cd93c1486eb200e4374103d876016e3b36080373bd758fc0f60</t>
+  </si>
+  <si>
+    <t>a5c860156e9ef8536f85dc49265640d8a398a15a7011e3211721d0395c36180c</t>
+  </si>
+  <si>
+    <t>12d31aa2bce4f6668966e434fd777e8e97f6d8f426991ec17e5c3be376551ac3</t>
   </si>
 </sst>
 </file>
@@ -697,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,6 +726,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -739,6 +745,9 @@
       </c>
       <c r="E2" s="2">
         <v>37108</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -758,6 +767,9 @@
       <c r="E3" s="2">
         <v>36712</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -776,6 +788,9 @@
       <c r="E4" s="2">
         <v>37104</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -793,6 +808,9 @@
       <c r="E5" s="2">
         <v>37368</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -810,8 +828,18 @@
       <c r="E6" s="2">
         <v>37632</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -820,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -844,7 +872,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -857,7 +885,7 @@
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -867,96 +895,103 @@
       <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
       <c r="G1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1234</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="str">
+        <f>G2&amp;C2</f>
+        <v>1234n5n7n1n8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
         <v>98</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="G3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" si="0">G3&amp;C3</f>
+        <v>1234h6h1h4h2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
         <v>99</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
       <c r="G4">
         <v>1234</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>1234o9o2o5o3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
       <c r="G5">
         <v>1234</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>1234a9a6a5a3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
       <c r="G6">
         <v>1234</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>1234a9a1a3a0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1124,10 +1159,10 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>